<commit_message>
Add latest set of flashcards
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - Römisches Recht - Klagen (JKU, Austria).xlsx
+++ b/flashcards/Memcode - Römisches Recht - Klagen (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>Question</t>
   </si>
@@ -19,18 +19,132 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was ist die actio ad supplendam legitimam?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Pflichtteilsberechtigter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbe&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilsergänzung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die querela inofficiosi testamenti?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Pflichtteilsberechtigter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erbe&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Aufhebung&lt;/strong&gt; des Testaments&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wegen &lt;strong&gt;Pflichtwidrigkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio testamento?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Bei &lt;/span&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Damnationslegat &lt;/em&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;-&amp;gt; nur &lt;/span&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;obligatorisch &lt;/em&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;berechtigt!&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Legatar &lt;/strong&gt;(Singularsukzessor)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbe&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(Universalsukzessor)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erfüllung &lt;/strong&gt;der &lt;strong&gt;Forderung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die rei vindicatio im Erbrecht? &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Bei welchem Legat?&lt;/li&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;li&gt;Was ist die Causa?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bei &lt;em&gt;Vindikationslegat &lt;/em&gt;-&amp;gt; &lt;em&gt;dinglich &lt;/em&gt;berechtigt!&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Legatar &lt;/strong&gt;(Singularsukzessor)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erbe&lt;/strong&gt; (Universalsukzessor)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Besitzer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Herausgabe&lt;/strong&gt; der Sache&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Causa&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;causa legati&lt;/em&gt;, &lt;strong&gt;abgeleitet &lt;/strong&gt;vom &lt;strong&gt;Erblasser&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio doli (Bereicherungsrechtlich) &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Arbiträrklausel&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beklagter kann &lt;strong&gt;Verurteilung entgehen&lt;/strong&gt;, wenn er noch &lt;strong&gt;während&lt;/strong&gt; &lt;strong&gt;Prozess&lt;/strong&gt; Schaden &lt;strong&gt;ersetzt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die condictio sine causa?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistung ohne&lt;/strong&gt; &lt;strong&gt;Grund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Nur subsidiär -&amp;gt; &lt;strong&gt;Auffangstatbestand&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio pretii? &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;li&gt;Unter welcher Bedingung?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nur vom &lt;strong&gt;Eigentümer&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Klagsabtretung &lt;/strong&gt;eventuell notwendig!&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Surrogat &lt;/strong&gt;(&lt;em&gt;Ersatz&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Herausgabe &lt;/strong&gt;des&lt;strong&gt; Kauferlöses&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Bedingung&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vindicatio unmöglich&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio ob iniustam causam?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leistung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;verbotener &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zweck&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio ob turpem causam?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leistung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;sittenwidriger &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zweck&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio ob causam datorum?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Leistung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zweck nicht&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; erreicht&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio causa finita?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Leistung, Wegfallen &lt;/strong&gt;des &lt;strong&gt;Grundes&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio indebiti?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Rückforderung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;irrtümliche&lt;/strong&gt; Leistung einer &lt;strong&gt;Nicht-Schuld&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio doli (deliktisch)?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;List / Betrug (nur subsidiär)&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Überlisteter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Betrüger&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio vi bonorum raptorum?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(171, 127, 242);"&gt;Raub&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Beraubter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Räuber&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;auf &lt;strong&gt;Buße &lt;/strong&gt;(&lt;em&gt;vierfach&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio iniuriarum?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(171, 127, 242);"&gt;Körperverletzung&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Opfer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Täter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schätzsumme &lt;/strong&gt;des &lt;strong&gt;Klägers&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio legis aquiliae?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Sachbeschädigung&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Geschädigter &lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;(Eigentümer)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Schädiger&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;auf &lt;strong&gt;Höchstwert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio furti?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Diebstahl&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Bestohlener &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dieb&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Buße&lt;/strong&gt; (&lt;em&gt;Doppelt &lt;/em&gt;oder &lt;em&gt;Vierfach&lt;/em&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die condictio furtiva?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Diebstahl&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Bestohlener &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dieb&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Rückgabe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Sachwert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio conducti &lt;span style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;beim &lt;/span&gt;&lt;em style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Werkvertrag&lt;/em&gt;?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Werkunternehmer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Besteller&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Werklohnzahlung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die actio commodati directa?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Bei commodatum - Leihe&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;(Verleiher)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Detentor &lt;/strong&gt;(Entlehner)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rückgabe &lt;/strong&gt;von &lt;strong&gt;exakt &lt;/strong&gt;dieser &lt;strong&gt;Sache&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nach &lt;em&gt;Zeitablauf&lt;/em&gt;, Bedingung, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Utilitätsprinzip -&amp;gt; &lt;em&gt;custodia&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gewöhnliche Erhaltungskosten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B. &lt;em&gt;Futter &lt;/em&gt;für ein Tier&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was ist die actio locati &lt;span style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;beim &lt;/span&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;Werkvertrag&lt;/em&gt;?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Besteller&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Werkunternehmer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Werkausführung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;(&lt;/span&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;faktischer&lt;/em&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;) &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erfolg&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die actio conducti &lt;span style="color: rgb(171, 127, 242); background-color: rgba(0, 0, 0, 0);"&gt;beim &lt;/span&gt;&lt;em style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Werkvertrag&lt;/em&gt;?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Werkunternehmer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Besteller&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Werklohnzahlung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die actio conducti &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;beim &lt;/span&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Dienstvertrag&lt;/em&gt;?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -115,18 +229,12 @@
     <t>&lt;p&gt;&lt;em&gt;Bei precarium - Bittleihe&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Precario&lt;/strong&gt; (Verleiher)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Prekarist &lt;/strong&gt;(Entlehner)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rückgabe&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;jederzeitiger &lt;/em&gt;Widerruf&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die actio commadati contraria?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was ist die actio commodati contraria?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Bei commodatum - Leihe&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Detentor &lt;/strong&gt;(Entlehner)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Gläubiger &lt;/strong&gt;(Verleiher)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;außerordentliche Aufwände&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei Schaden &lt;em&gt;durch die Sache&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was ist die actio commadati directa?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Bei commodatum - Leihe&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Von&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gläubiger &lt;/strong&gt;(Verleiher)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Gegen&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Detentor &lt;/strong&gt;(Entlehner)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Auf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rückgabe &lt;/strong&gt;von &lt;strong&gt;exakt &lt;/strong&gt;dieser &lt;strong&gt;Sache&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nach &lt;em&gt;Zeitablauf&lt;/em&gt;, Bedingung, ...&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Schadenersatz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Utilitätsprinzip -&amp;gt; &lt;em&gt;custodia&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gewöhnliche Erhaltungskosten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;z.B. &lt;em&gt;Futter &lt;/em&gt;für ein Tier&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;Was ist die actio certae creditae pecuniae?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem gegen wen?&lt;/li&gt;&lt;li&gt;Welches Ziel?&lt;/li&gt;&lt;li&gt;Welche Einreden gibt es?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
@@ -238,7 +346,7 @@
     <t>&lt;p&gt;Was ist die exceptio iusti dominii?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem?&lt;/li&gt;&lt;li&gt;gegen welche Klage?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;bonitarischen Eingetümer &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gegen jeden schlechter Berechtigten (z.B.: EB)&lt;/li&gt;&lt;li&gt;gegen die actio publiciana &lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;bonitarischen Eigentümer &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gegen jeden schlechter Berechtigten (z.B.: EB)&lt;/li&gt;&lt;li&gt;gegen die actio publiciana&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist die &lt;strong&gt;replicatio &lt;/strong&gt;rei vendita et traditae?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Von wem?&lt;/li&gt;&lt;li&gt;gegen welche Klage?&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
@@ -664,7 +772,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B62"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -1022,6 +1130,150 @@
         <v>87</v>
       </c>
     </row>
+    <row r="45" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>